<commit_message>
HP : Progress in report
</commit_message>
<xml_diff>
--- a/TP3/MaDUM.xlsx
+++ b/TP3/MaDUM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakim\Documents\Polytechnique\H20\LOG3430\TPs\Test_LOG3430-\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D50ED77-A874-4E29-AD52-75977B3C5EDB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65912316-43C6-46A9-A19A-345191898C4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B62AB78A-C09B-4AFF-BAD9-62F27D279AE3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
   <si>
     <t>weight</t>
   </si>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AEBD75-01E7-4A96-B4F6-1065DBB4A301}">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,6 +596,128 @@
       </c>
       <c r="H7" s="2"/>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
RZ : Progress in report and tests
</commit_message>
<xml_diff>
--- a/TP3/MaDUM.xlsx
+++ b/TP3/MaDUM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakim\Documents\Polytechnique\H20\LOG3430\TPs\Test_LOG3430-\TP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romaz\Desktop\Test_LOG3430-\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65912316-43C6-46A9-A19A-345191898C4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC76E15-FC24-4C6E-B0EA-C0ACAD20E823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B62AB78A-C09B-4AFF-BAD9-62F27D279AE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B62AB78A-C09B-4AFF-BAD9-62F27D279AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="16">
   <si>
     <t>weight</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>__encode_tree</t>
+  </si>
+  <si>
+    <t>encode_tree</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -451,16 +454,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AEBD75-01E7-4A96-B4F6-1065DBB4A301}">
   <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="15.6328125" customWidth="1"/>
+    <col min="2" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -484,7 +487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +505,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -526,7 +529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -550,7 +553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -574,7 +577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -596,7 +599,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -608,7 +611,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>7</v>
@@ -620,7 +623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +639,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -660,7 +663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -680,7 +683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -700,7 +703,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
HP : WIP icant live
</commit_message>
<xml_diff>
--- a/TP3/MaDUM.xlsx
+++ b/TP3/MaDUM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romaz\Desktop\Test_LOG3430-\TP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakim\Documents\Polytechnique\H20\LOG3430\TPs\Test_LOG3430-\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC76E15-FC24-4C6E-B0EA-C0ACAD20E823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C82C56-3A61-4EAA-9F36-EAE3338A20E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B62AB78A-C09B-4AFF-BAD9-62F27D279AE3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B62AB78A-C09B-4AFF-BAD9-62F27D279AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="16">
   <si>
     <t>weight</t>
   </si>
@@ -94,12 +94,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -129,13 +135,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -156,7 +165,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -452,18 +461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AEBD75-01E7-4A96-B4F6-1065DBB4A301}">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="11" width="15.5703125" customWidth="1"/>
+    <col min="2" max="16" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -487,7 +496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +514,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -529,7 +538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -553,7 +562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -577,7 +586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -599,7 +608,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -622,8 +631,30 @@
       <c r="H10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="3"/>
+      <c r="J10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,8 +669,22 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -662,8 +707,30 @@
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -682,8 +749,26 @@
       <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -702,8 +787,26 @@
       <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -720,6 +823,134 @@
         <v>13</v>
       </c>
       <c r="H15" s="2"/>
+      <c r="I15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RZ : Finished all MaDUM tests for Huffman
</commit_message>
<xml_diff>
--- a/TP3/MaDUM.xlsx
+++ b/TP3/MaDUM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakim\Documents\Polytechnique\H20\LOG3430\TPs\Test_LOG3430-\TP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romaz\Desktop\Test_LOG3430-\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C82C56-3A61-4EAA-9F36-EAE3338A20E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1CEDC5-7E21-4852-945E-B69C92F5BDD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B62AB78A-C09B-4AFF-BAD9-62F27D279AE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B62AB78A-C09B-4AFF-BAD9-62F27D279AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,16 +463,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AEBD75-01E7-4A96-B4F6-1065DBB4A301}">
   <dimension ref="A2:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="16" width="15.54296875" customWidth="1"/>
+    <col min="2" max="16" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -496,7 +496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -538,7 +538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -562,7 +562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -586,7 +586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -608,7 +608,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -654,7 +654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +684,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -713,24 +713,24 @@
       <c r="J12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="K12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O12" s="1"/>
-      <c r="P12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P12" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -755,20 +755,20 @@
       <c r="J13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -793,20 +793,20 @@
       <c r="J14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P14" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -829,18 +829,18 @@
       <c r="J15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1" t="s">
+      <c r="O15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="P15" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
         <v>10</v>
@@ -861,7 +861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +876,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -897,7 +897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -916,7 +916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -935,7 +935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>